<commit_message>
Cheat Bar functions great
Got the bar to finally view all data and locked in the connections
</commit_message>
<xml_diff>
--- a/data/items/itemsWORKBOOK.xlsx
+++ b/data/items/itemsWORKBOOK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\Projects\Psyokin\data\items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A57752-5172-4DA9-9EB3-B2E064DD8DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24903AC6-D4C7-4C70-A0C2-A65837121469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2625" windowWidth="33495" windowHeight="17940" tabRatio="793" activeTab="5" xr2:uid="{3DC06797-DF42-4A20-B1D4-AE1AB78E8A9F}"/>
+    <workbookView xWindow="1965" yWindow="1935" windowWidth="35040" windowHeight="17940" tabRatio="793" activeTab="6" xr2:uid="{3DC06797-DF42-4A20-B1D4-AE1AB78E8A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="22" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="211">
   <si>
     <t>item_id</t>
   </si>
@@ -643,6 +643,84 @@
   </si>
   <si>
     <t>"A metal bracelet with 2 slots. Very sturdy."</t>
+  </si>
+  <si>
+    <t>SIG_002</t>
+  </si>
+  <si>
+    <t>Water Sigil</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Splash a foe.</t>
+  </si>
+  <si>
+    <t>A basic Water sigil that deals minor water damage to a single enemy.</t>
+  </si>
+  <si>
+    <t>Deal 30 Water DMG</t>
+  </si>
+  <si>
+    <t>SIG_003</t>
+  </si>
+  <si>
+    <t>SIG_004</t>
+  </si>
+  <si>
+    <t>SIG_005</t>
+  </si>
+  <si>
+    <t>SIG_006</t>
+  </si>
+  <si>
+    <t>Earth Sigil</t>
+  </si>
+  <si>
+    <t>Air Sigil</t>
+  </si>
+  <si>
+    <t>Void Sigil</t>
+  </si>
+  <si>
+    <t>Data Sigil</t>
+  </si>
+  <si>
+    <t>It's pocket sand.</t>
+  </si>
+  <si>
+    <t>Blow them away.</t>
+  </si>
+  <si>
+    <t>Don't stare too long.</t>
+  </si>
+  <si>
+    <t>Give your foe a 404 erorr.</t>
+  </si>
+  <si>
+    <t>A basic Earth sigil that deals minor earth damage to a single enemy.</t>
+  </si>
+  <si>
+    <t>A basic Air sigil that deals minor air damage to a single enemy.</t>
+  </si>
+  <si>
+    <t>A basic Void sigil that deals minor void damage to a single enemy.</t>
+  </si>
+  <si>
+    <t>A basic Data sigil that deals minor data damage to a single enemy.</t>
+  </si>
+  <si>
+    <t>Deal 30 Earth DMG</t>
+  </si>
+  <si>
+    <t>Deal 30 Air DMG</t>
+  </si>
+  <si>
+    <t>Deal 30 Void DMG</t>
+  </si>
+  <si>
+    <t>Deal 30 Data DMG</t>
   </si>
 </sst>
 </file>
@@ -1685,8 +1763,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E05CB7CE-2FCC-4455-89EC-7620263AB97F}" name="tblSigils" displayName="tblSigils" ref="A1:BA2" totalsRowShown="0">
-  <autoFilter ref="A1:BA2" xr:uid="{6B45D362-841E-4115-BA5F-5ADB6CDEE454}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E05CB7CE-2FCC-4455-89EC-7620263AB97F}" name="tblSigils" displayName="tblSigils" ref="A1:BA7" totalsRowShown="0">
+  <autoFilter ref="A1:BA7" xr:uid="{6B45D362-841E-4115-BA5F-5ADB6CDEE454}"/>
   <tableColumns count="53">
     <tableColumn id="1" xr3:uid="{18A53ACC-FC62-418F-8BB5-D7F51FEAD9D5}" name="item_id"/>
     <tableColumn id="2" xr3:uid="{20C6EDB1-F572-414E-816D-12291DE3A678}" name="name"/>
@@ -2249,7 +2327,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B1308D-EBD5-4B85-B543-34EF1A52AC7F}">
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA19"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AF29" sqref="AF29"/>
@@ -2271,7 +2349,7 @@
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="str" cm="1">
-        <f t="array" ref="A1:BA14">_xlfn.LET(_xlpm.W, tblWeapons[], _xlpm.A, tblArmor[], _xlpm.H, tblHeadwear[],_xlpm.F, tblFootwear[],_xlpm.B, tblBracelets[],_xlpm.S, tblSigils[],_xlpm.C, tblConsumables[],_xlpm.M, tblMaterials[],_xlpm.G, tblGifts[],_xlpm.K, tblKeys[],_xlpm.Data, _xlfn.VSTACK(_xlpm.W, _xlpm.A, _xlpm.H,_xlpm.F,_xlpm.B,_xlpm.S,_xlpm.C,_xlpm.M,_xlpm.G,_xlpm.K),_xlpm.NonBlank, _xlfn._xlws.FILTER(_xlpm.Data, _xlfn.BYROW(_xlpm.Data, _xlfn.LAMBDA(_xlpm.r, COUNTA(_xlpm.r)&gt;0))),_xlfn.VSTACK(tblWeapons[#Headers], _xlpm.NonBlank))</f>
+        <f t="array" ref="A1:BA19">_xlfn.LET(_xlpm.W, tblWeapons[], _xlpm.A, tblArmor[], _xlpm.H, tblHeadwear[],_xlpm.F, tblFootwear[],_xlpm.B, tblBracelets[],_xlpm.S, tblSigils[],_xlpm.C, tblConsumables[],_xlpm.M, tblMaterials[],_xlpm.G, tblGifts[],_xlpm.K, tblKeys[],_xlpm.Data, _xlfn.VSTACK(_xlpm.W, _xlpm.A, _xlpm.H,_xlpm.F,_xlpm.B,_xlpm.S,_xlpm.C,_xlpm.M,_xlpm.G,_xlpm.K),_xlpm.NonBlank, _xlfn._xlws.FILTER(_xlpm.Data, _xlfn.BYROW(_xlpm.Data, _xlfn.LAMBDA(_xlpm.r, COUNTA(_xlpm.r)&gt;0))),_xlfn.VSTACK(tblWeapons[#Headers], _xlpm.NonBlank))</f>
         <v>item_id</v>
       </c>
       <c r="B1" s="2" t="str">
@@ -3721,16 +3799,16 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
-        <v>CON_001</v>
+        <v>SIG_002</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Health Drink</v>
+        <v>Water Sigil</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Consumables</v>
+        <v>Sigils</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>none</v>
+        <v>Sigil</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>Common</v>
@@ -3739,10 +3817,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="H10" s="4">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="I10" s="4">
         <v>1</v>
@@ -3751,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="4">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
@@ -3760,79 +3838,79 @@
         <v>0</v>
       </c>
       <c r="N10" s="4" t="str">
-        <v>"Restores a bit of health."</v>
+        <v>Splash a foe.</v>
       </c>
       <c r="O10" s="4" t="str">
-        <v>"A basic sports drink that restores 50 HP to one ally."</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>0</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0</v>
-      </c>
-      <c r="S10" s="4">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <v>0</v>
-      </c>
-      <c r="U10" s="4">
-        <v>0</v>
-      </c>
-      <c r="V10" s="4">
-        <v>0</v>
-      </c>
-      <c r="W10" s="4">
-        <v>0</v>
-      </c>
-      <c r="X10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="4">
-        <v>0</v>
+        <v>A basic Water sigil that deals minor water damage to a single enemy.</v>
+      </c>
+      <c r="P10" s="4" t="str">
+        <v>water</v>
+      </c>
+      <c r="Q10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="R10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="S10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="T10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="U10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="V10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="W10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="X10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AD10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AE10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AF10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AG10" s="4" t="str">
+        <v>Water</v>
+      </c>
+      <c r="AH10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AI10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AJ10" s="4" t="str">
+        <v>null</v>
       </c>
       <c r="AK10" s="4" t="str">
-        <v>both</v>
+        <v>battle</v>
       </c>
       <c r="AL10" s="4" t="str">
-        <v>Ally</v>
+        <v>Enemy</v>
       </c>
       <c r="AM10" s="4">
         <v>0</v>
@@ -3841,22 +3919,22 @@
         <v>0</v>
       </c>
       <c r="AO10" s="4" t="str">
-        <v>"Heal 50 HP"</v>
-      </c>
-      <c r="AP10" s="4" t="str">
-        <v>"Heal 50 HP"</v>
+        <v>Deal 30 Water DMG</v>
+      </c>
+      <c r="AP10" s="4">
+        <v>0</v>
       </c>
       <c r="AQ10" s="4">
         <v>0</v>
       </c>
       <c r="AR10" s="4" t="str">
-        <v>none</v>
-      </c>
-      <c r="AS10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="4">
-        <v>0</v>
+        <v>null</v>
+      </c>
+      <c r="AS10" s="4" t="str">
+        <v>null</v>
+      </c>
+      <c r="AT10" s="4" t="str">
+        <v>null</v>
       </c>
       <c r="AU10" s="4">
         <v>0</v>
@@ -3876,22 +3954,22 @@
       <c r="AZ10" s="4">
         <v>0</v>
       </c>
-      <c r="BA10" s="4">
-        <v>0</v>
+      <c r="BA10" s="4" t="str">
+        <v>null</v>
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
-        <v>CON_002</v>
+        <v>SIG_003</v>
       </c>
       <c r="B11" s="4" t="str">
-        <v>Mind Drink</v>
+        <v>Earth Sigil</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>Consumables</v>
+        <v>Sigils</v>
       </c>
       <c r="D11" s="4" t="str">
-        <v>none</v>
+        <v>Sigil</v>
       </c>
       <c r="E11" s="4" t="str">
         <v>Common</v>
@@ -3900,11 +3978,11 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
+        <v>120</v>
+      </c>
+      <c r="H11" s="4">
         <v>60</v>
       </c>
-      <c r="H11" s="4">
-        <v>30</v>
-      </c>
       <c r="I11" s="4">
         <v>1</v>
       </c>
@@ -3912,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="4">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
@@ -3921,13 +3999,13 @@
         <v>0</v>
       </c>
       <c r="N11" s="4" t="str">
-        <v>"Restores a some mind points."</v>
+        <v>It's pocket sand.</v>
       </c>
       <c r="O11" s="4" t="str">
-        <v>"A basic sports drink that restores 30 MP to one ally."</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0</v>
+        <v>A basic Earth sigil that deals minor earth damage to a single enemy.</v>
+      </c>
+      <c r="P11" s="4" t="str">
+        <v>earth</v>
       </c>
       <c r="Q11" s="4">
         <v>0</v>
@@ -3977,8 +4055,8 @@
       <c r="AF11" s="4">
         <v>0</v>
       </c>
-      <c r="AG11" s="4">
-        <v>0</v>
+      <c r="AG11" s="4" t="str">
+        <v>Earth</v>
       </c>
       <c r="AH11" s="4">
         <v>0</v>
@@ -3990,10 +4068,10 @@
         <v>0</v>
       </c>
       <c r="AK11" s="4" t="str">
-        <v>both</v>
+        <v>battle</v>
       </c>
       <c r="AL11" s="4" t="str">
-        <v>Ally</v>
+        <v>Enemy</v>
       </c>
       <c r="AM11" s="4">
         <v>0</v>
@@ -4002,16 +4080,16 @@
         <v>0</v>
       </c>
       <c r="AO11" s="4" t="str">
-        <v>"Heal 30 MP"</v>
-      </c>
-      <c r="AP11" s="4" t="str">
-        <v>"Heal 30 MP"</v>
+        <v>Deal 30 Earth DMG</v>
+      </c>
+      <c r="AP11" s="4">
+        <v>0</v>
       </c>
       <c r="AQ11" s="4">
         <v>0</v>
       </c>
-      <c r="AR11" s="4" t="str">
-        <v>none</v>
+      <c r="AR11" s="4">
+        <v>0</v>
       </c>
       <c r="AS11" s="4">
         <v>0</v>
@@ -4043,16 +4121,16 @@
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
-        <v>MAT_001</v>
+        <v>SIG_004</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Rock</v>
+        <v>Air Sigil</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Materials</v>
+        <v>Sigils</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>none</v>
+        <v>Sigil</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>Common</v>
@@ -4061,10 +4139,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="H12" s="4">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="I12" s="4">
         <v>1</v>
@@ -4073,22 +4151,22 @@
         <v>1</v>
       </c>
       <c r="K12" s="4">
-        <v>99</v>
-      </c>
-      <c r="L12" s="4" t="str">
-        <v>lowland_node</v>
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
       </c>
       <c r="N12" s="4" t="str">
-        <v>"Basic crafting material."</v>
+        <v>Blow them away.</v>
       </c>
       <c r="O12" s="4" t="str">
-        <v>"A small, common stone used in early-game crafting recipes."</v>
-      </c>
-      <c r="P12" s="4">
-        <v>0</v>
+        <v>A basic Air sigil that deals minor air damage to a single enemy.</v>
+      </c>
+      <c r="P12" s="4" t="str">
+        <v>air</v>
       </c>
       <c r="Q12" s="4">
         <v>0</v>
@@ -4138,8 +4216,8 @@
       <c r="AF12" s="4">
         <v>0</v>
       </c>
-      <c r="AG12" s="4">
-        <v>0</v>
+      <c r="AG12" s="4" t="str">
+        <v>Air</v>
       </c>
       <c r="AH12" s="4">
         <v>0</v>
@@ -4150,11 +4228,11 @@
       <c r="AJ12" s="4">
         <v>0</v>
       </c>
-      <c r="AK12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="4">
-        <v>0</v>
+      <c r="AK12" s="4" t="str">
+        <v>battle</v>
+      </c>
+      <c r="AL12" s="4" t="str">
+        <v>Enemy</v>
       </c>
       <c r="AM12" s="4">
         <v>0</v>
@@ -4162,8 +4240,8 @@
       <c r="AN12" s="4">
         <v>0</v>
       </c>
-      <c r="AO12" s="4">
-        <v>0</v>
+      <c r="AO12" s="4" t="str">
+        <v>Deal 30 Air DMG</v>
       </c>
       <c r="AP12" s="4">
         <v>0</v>
@@ -4204,16 +4282,16 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
-        <v>GIF_001</v>
+        <v>SIG_005</v>
       </c>
       <c r="B13" s="4" t="str">
-        <v>Earing</v>
+        <v>Void Sigil</v>
       </c>
       <c r="C13" s="4" t="str">
-        <v>Gifts</v>
+        <v>Sigils</v>
       </c>
       <c r="D13" s="4" t="str">
-        <v>none</v>
+        <v>Sigil</v>
       </c>
       <c r="E13" s="4" t="str">
         <v>Common</v>
@@ -4225,7 +4303,7 @@
         <v>120</v>
       </c>
       <c r="H13" s="4">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
@@ -4234,7 +4312,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
@@ -4243,13 +4321,13 @@
         <v>0</v>
       </c>
       <c r="N13" s="4" t="str">
-        <v>"Simple silver earring."</v>
+        <v>Don't stare too long.</v>
       </c>
       <c r="O13" s="4" t="str">
-        <v>"A modest silver earring; some circle members love small accessories."</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
+        <v>A basic Void sigil that deals minor void damage to a single enemy.</v>
+      </c>
+      <c r="P13" s="4" t="str">
+        <v>data</v>
       </c>
       <c r="Q13" s="4">
         <v>0</v>
@@ -4299,8 +4377,8 @@
       <c r="AF13" s="4">
         <v>0</v>
       </c>
-      <c r="AG13" s="4">
-        <v>0</v>
+      <c r="AG13" s="4" t="str">
+        <v>Data</v>
       </c>
       <c r="AH13" s="4">
         <v>0</v>
@@ -4311,11 +4389,11 @@
       <c r="AJ13" s="4">
         <v>0</v>
       </c>
-      <c r="AK13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="4">
-        <v>0</v>
+      <c r="AK13" s="4" t="str">
+        <v>battle</v>
+      </c>
+      <c r="AL13" s="4" t="str">
+        <v>Enemy</v>
       </c>
       <c r="AM13" s="4">
         <v>0</v>
@@ -4323,8 +4401,8 @@
       <c r="AN13" s="4">
         <v>0</v>
       </c>
-      <c r="AO13" s="4">
-        <v>0</v>
+      <c r="AO13" s="4" t="str">
+        <v>Deal 30 Void DMG</v>
       </c>
       <c r="AP13" s="4">
         <v>0</v>
@@ -4359,168 +4437,973 @@
       <c r="AZ13" s="4">
         <v>0</v>
       </c>
-      <c r="BA13" s="4" t="str">
-        <v>Fashion</v>
+      <c r="BA13" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
+        <v>SIG_006</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <v>Data Sigil</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <v>Sigils</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <v>Sigil</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <v>Common</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>120</v>
+      </c>
+      <c r="H14" s="4">
+        <v>60</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4" t="str">
+        <v>Give your foe a 404 erorr.</v>
+      </c>
+      <c r="O14" s="4" t="str">
+        <v>A basic Data sigil that deals minor data damage to a single enemy.</v>
+      </c>
+      <c r="P14" s="4" t="str">
+        <v>void</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0</v>
+      </c>
+      <c r="T14" s="4">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0</v>
+      </c>
+      <c r="V14" s="4">
+        <v>0</v>
+      </c>
+      <c r="W14" s="4">
+        <v>0</v>
+      </c>
+      <c r="X14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="4" t="str">
+        <v>Void</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="4" t="str">
+        <v>battle</v>
+      </c>
+      <c r="AL14" s="4" t="str">
+        <v>Enemy</v>
+      </c>
+      <c r="AM14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="4" t="str">
+        <v>Deal 30 Data DMG</v>
+      </c>
+      <c r="AP14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ14" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str">
+        <v>CON_001</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <v>Health Drink</v>
+      </c>
+      <c r="C15" s="4" t="str">
+        <v>Consumables</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <v>Common</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>30</v>
+      </c>
+      <c r="H15" s="4">
+        <v>15</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>99</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4" t="str">
+        <v>"Restores a bit of health."</v>
+      </c>
+      <c r="O15" s="4" t="str">
+        <v>"A basic sports drink that restores 50 HP to one ally."</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0</v>
+      </c>
+      <c r="V15" s="4">
+        <v>0</v>
+      </c>
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="4" t="str">
+        <v>both</v>
+      </c>
+      <c r="AL15" s="4" t="str">
+        <v>Ally</v>
+      </c>
+      <c r="AM15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="4" t="str">
+        <v>"Heal 50 HP"</v>
+      </c>
+      <c r="AP15" s="4" t="str">
+        <v>"Heal 50 HP"</v>
+      </c>
+      <c r="AQ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="AS15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <v>CON_002</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <v>Mind Drink</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <v>Consumables</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <v>Common</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>60</v>
+      </c>
+      <c r="H16" s="4">
+        <v>30</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>99</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4" t="str">
+        <v>"Restores a some mind points."</v>
+      </c>
+      <c r="O16" s="4" t="str">
+        <v>"A basic sports drink that restores 30 MP to one ally."</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+      <c r="V16" s="4">
+        <v>0</v>
+      </c>
+      <c r="W16" s="4">
+        <v>0</v>
+      </c>
+      <c r="X16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="4" t="str">
+        <v>both</v>
+      </c>
+      <c r="AL16" s="4" t="str">
+        <v>Ally</v>
+      </c>
+      <c r="AM16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="4" t="str">
+        <v>"Heal 30 MP"</v>
+      </c>
+      <c r="AP16" s="4" t="str">
+        <v>"Heal 30 MP"</v>
+      </c>
+      <c r="AQ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="AS16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str">
+        <v>MAT_001</v>
+      </c>
+      <c r="B17" s="4" t="str">
+        <v>Rock</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <v>Materials</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <v>Common</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1</v>
+      </c>
+      <c r="J17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>99</v>
+      </c>
+      <c r="L17" s="4" t="str">
+        <v>lowland_node</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4" t="str">
+        <v>"Basic crafting material."</v>
+      </c>
+      <c r="O17" s="4" t="str">
+        <v>"A small, common stone used in early-game crafting recipes."</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>0</v>
+      </c>
+      <c r="V17" s="4">
+        <v>0</v>
+      </c>
+      <c r="W17" s="4">
+        <v>0</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
+        <v>GIF_001</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <v>Earing</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <v>Gifts</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <v>none</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <v>Common</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>120</v>
+      </c>
+      <c r="H18" s="4">
+        <v>30</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
+      <c r="J18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4" t="str">
+        <v>"Simple silver earring."</v>
+      </c>
+      <c r="O18" s="4" t="str">
+        <v>"A modest silver earring; some circle members love small accessories."</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+      <c r="V18" s="4">
+        <v>0</v>
+      </c>
+      <c r="W18" s="4">
+        <v>0</v>
+      </c>
+      <c r="X18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="4" t="str">
+        <v>Fashion</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="str">
         <v>KEY_001</v>
       </c>
-      <c r="B14" s="4" t="str">
+      <c r="B19" s="4" t="str">
         <v>Family Picture</v>
       </c>
-      <c r="C14" s="4" t="str">
+      <c r="C19" s="4" t="str">
         <v>Key</v>
       </c>
-      <c r="D14" s="4" t="str">
+      <c r="D19" s="4" t="str">
         <v>none</v>
       </c>
-      <c r="E14" s="4" t="str">
+      <c r="E19" s="4" t="str">
         <v>Legendary</v>
       </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>1</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4" t="str">
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4" t="str">
         <v>"A worn family photo."</v>
       </c>
-      <c r="O14" s="4" t="str">
+      <c r="O19" s="4" t="str">
         <v>"You can’t bring yourself to part with it. A key story keepsake."</v>
       </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>0</v>
-      </c>
-      <c r="R14" s="4">
-        <v>0</v>
-      </c>
-      <c r="S14" s="4">
-        <v>0</v>
-      </c>
-      <c r="T14" s="4">
-        <v>0</v>
-      </c>
-      <c r="U14" s="4">
-        <v>0</v>
-      </c>
-      <c r="V14" s="4">
-        <v>0</v>
-      </c>
-      <c r="W14" s="4">
-        <v>0</v>
-      </c>
-      <c r="X14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="4" t="str">
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <v>0</v>
+      </c>
+      <c r="V19" s="4">
+        <v>0</v>
+      </c>
+      <c r="W19" s="4">
+        <v>0</v>
+      </c>
+      <c r="X19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="4" t="str">
         <v>Family</v>
       </c>
-      <c r="AV14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA14" s="4">
+      <c r="AV19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7223,7 +8106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5BD1EB-EDA5-486E-B061-143EABAA45C1}">
   <dimension ref="A1:BA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
@@ -7602,10 +8485,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782F3198-6067-4BC9-81A1-E2DEF4C07151}">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7876,75 +8759,425 @@
         <v>159</v>
       </c>
     </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O3" t="s">
+        <v>189</v>
+      </c>
+      <c r="P3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>187</v>
+      </c>
+      <c r="R3" t="s">
+        <v>187</v>
+      </c>
+      <c r="S3" t="s">
+        <v>187</v>
+      </c>
+      <c r="T3" t="s">
+        <v>187</v>
+      </c>
+      <c r="U3" t="s">
+        <v>187</v>
+      </c>
+      <c r="V3" t="s">
+        <v>187</v>
+      </c>
+      <c r="W3" t="s">
+        <v>187</v>
+      </c>
+      <c r="X3" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>199</v>
+      </c>
+      <c r="O4" t="s">
+        <v>203</v>
+      </c>
+      <c r="P4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O5" t="s">
+        <v>204</v>
+      </c>
+      <c r="P5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O6" t="s">
+        <v>205</v>
+      </c>
+      <c r="P6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7">
+        <v>120</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O7" t="s">
+        <v>206</v>
+      </c>
+      <c r="P7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="21">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B2" xr:uid="{7FDB170D-1CF7-4DD6-9002-ECB1ABD45887}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{7FDB170D-1CF7-4DD6-9002-ECB1ABD45887}">
       <formula1>1</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C2" xr:uid="{E2BA580E-F9C0-4B1D-B518-4CB1589D57DD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C7" xr:uid="{E2BA580E-F9C0-4B1D-B518-4CB1589D57DD}">
       <formula1>list_category</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2" xr:uid="{87CFCB66-E17C-462F-9F6E-80C2D4B16AAA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D7" xr:uid="{87CFCB66-E17C-462F-9F6E-80C2D4B16AAA}">
       <formula1>list_equip_slot</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E2" xr:uid="{72728A0A-67E4-407A-94E5-10426650303B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E7" xr:uid="{72728A0A-67E4-407A-94E5-10426650303B}">
       <formula1>list_rarity</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I2 R1:U2 X1:Z2 AB1:AB2 AD1:AD2 AM1:AN2 AQ1:AQ2 AT1:AT2 AG1" xr:uid="{9599E056-76B1-4487-A2C7-284AC0AD44F8}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J2 AE1:AE2" xr:uid="{DD3F6C56-F803-4BB7-BE4B-AC7B7EE9AB6A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE7 J1:J7" xr:uid="{DD3F6C56-F803-4BB7-BE4B-AC7B7EE9AB6A}">
       <formula1>list_boolean</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K2" xr:uid="{8476F686-FE2B-4F16-B57C-1E61864F89C4}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K7" xr:uid="{8476F686-FE2B-4F16-B57C-1E61864F89C4}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2" xr:uid="{2B917806-5C7A-4C77-B347-B693613401FC}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N7" xr:uid="{2B917806-5C7A-4C77-B347-B693613401FC}">
       <formula1>120</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O2" xr:uid="{2AB0490B-1422-4838-9861-F0C5E3B266A6}">
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O7" xr:uid="{2AB0490B-1422-4838-9861-F0C5E3B266A6}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P2" xr:uid="{20A400E7-5604-4EF8-8A3A-D33E7EB60E93}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P7" xr:uid="{20A400E7-5604-4EF8-8A3A-D33E7EB60E93}">
       <formula1>list_mind_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q2" xr:uid="{0050C0FA-9E7D-43AA-964F-9281E5A99A60}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q7" xr:uid="{0050C0FA-9E7D-43AA-964F-9281E5A99A60}">
       <formula1>list_watk_type</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V2" xr:uid="{59070A2B-9E48-49E7-96A6-117072745A41}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V7" xr:uid="{59070A2B-9E48-49E7-96A6-117072745A41}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA2" xr:uid="{1190C7E3-9346-4A86-8AB8-A87724C921D9}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA7" xr:uid="{1190C7E3-9346-4A86-8AB8-A87724C921D9}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC1:AC2" xr:uid="{6B5C7E16-9BA0-4960-8B83-29C18C5BCFDD}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC1:AC7" xr:uid="{6B5C7E16-9BA0-4960-8B83-29C18C5BCFDD}">
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1:AF2" xr:uid="{47F36D5E-BDCF-48E7-AC28-2213E6686B40}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1:AF7" xr:uid="{47F36D5E-BDCF-48E7-AC28-2213E6686B40}">
       <formula1>0</formula1>
       <formula2>7</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG1:AG2" xr:uid="{031D9C6E-C01C-4C68-BDBD-E68D66606D43}">
       <formula1>list_sigil_school</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK1:AK2" xr:uid="{488DDBB8-70EE-4731-80F1-5CB77F334FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK1:AK7" xr:uid="{488DDBB8-70EE-4731-80F1-5CB77F334FBF}">
       <formula1>list_use_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL1:AL2" xr:uid="{5F258C43-3936-483E-81B6-C8C888C88F2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL1:AL7" xr:uid="{5F258C43-3936-483E-81B6-C8C888C88F2B}">
       <formula1>list_targeting</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR1:AR2" xr:uid="{CFFEA656-93FB-4B77-B9BB-87A43AD29CB2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR1:AR7" xr:uid="{CFFEA656-93FB-4B77-B9BB-87A43AD29CB2}">
       <formula1>list_capture_type</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW1:AW2" xr:uid="{665038BC-260A-429B-9D56-C283B2C349AC}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW1:AW7" xr:uid="{665038BC-260A-429B-9D56-C283B2C349AC}">
       <formula1>1</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA1:BA2" xr:uid="{5CFEEE6B-C42D-4E8C-9652-05F446023962}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA1:BA7" xr:uid="{5CFEEE6B-C42D-4E8C-9652-05F446023962}">
       <formula1>list_gift_type</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>